<commit_message>
fix: :ambulance: Fechas inconsistentes en PLOVMAE 2019/05
</commit_message>
<xml_diff>
--- a/apps/load_data/2019/05/PLMOVMAE.xlsx
+++ b/apps/load_data/2019/05/PLMOVMAE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NOMBRADOS -2019\HHY0519\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drey\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1502E783-940D-4828-B5CC-828D031E9A6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F130D19E-F570-4AC3-91C4-E448E072B241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10951,8 +10951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CI293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="J295" sqref="J295"/>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="Q293" sqref="Q293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10970,10 +10970,10 @@
     <col min="11" max="11" width="45.7109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="1.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="1.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="15.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="1.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="8.7109375" customWidth="1"/>
     <col min="20" max="20" width="16.7109375" style="1" customWidth="1"/>
@@ -63467,7 +63467,7 @@
       <c r="P290" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q290" s="5">
+      <c r="Q290" s="3">
         <v>27862</v>
       </c>
       <c r="R290" s="4" t="s">
@@ -63688,7 +63688,7 @@
       <c r="P291" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q291" s="5">
+      <c r="Q291" s="3">
         <v>29411</v>
       </c>
       <c r="R291" s="4" t="s">
@@ -63902,7 +63902,7 @@
       <c r="P292" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q292" s="5">
+      <c r="Q292" s="3">
         <v>29181</v>
       </c>
       <c r="R292" s="4" t="s">
@@ -64115,7 +64115,7 @@
       <c r="P293" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q293" s="5">
+      <c r="Q293" s="3">
         <v>23180</v>
       </c>
       <c r="R293" s="4" t="s">

</xml_diff>